<commit_message>
Added the sprint2 to the scrum board
</commit_message>
<xml_diff>
--- a/project/phase2/Scrum Board.xlsx
+++ b/project/phase2/Scrum Board.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC Master\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049B8271-166D-449A-AE92-E7C60DC51F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A32E7A-D6AC-4AF1-B4EE-F7A9ACA7CF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{74F4B266-3A8B-474A-B578-0D138B65883D}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{74F4B266-3A8B-474A-B578-0D138B65883D}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Sprint 4</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Tiago, Pedro, and João should analyze the code and identify classes and data Structures important to implement trash.</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Each member should read the code and analize the functionalities already implemented</t>
+  </si>
+  <si>
+    <t>The members should discuss the features</t>
   </si>
 </sst>
 </file>
@@ -101,10 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -123,7 +133,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -419,51 +429,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574BCB64-20F7-4A5A-B2B6-667020A6BF47}">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="105.6640625" customWidth="1"/>
+    <col min="2" max="2" width="105.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>